<commit_message>
Added map authors, Added map geometry for reckoning maps.
</commit_message>
<xml_diff>
--- a/Reference_Info/Texture replacements.xlsx
+++ b/Reference_Info/Texture replacements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stevenconnell\OneDrive - CTS Group Pty Ltd\Documents\GitHub\BD64maps_v2.666\Reference_Info\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Connell\Documents\GitHub\BD64-VoH_maps\Reference_Info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A36CD00-29A6-49CA-8B96-658E926258B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E9186E-56CC-4A5E-A58A-DB34806DA49B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A567E191-AF02-4B5D-A98D-30E219FAA09A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A567E191-AF02-4B5D-A98D-30E219FAA09A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,15 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="192">
   <si>
     <t>NEW50</t>
   </si>
@@ -520,6 +523,87 @@
   </si>
   <si>
     <t>TILEF504</t>
+  </si>
+  <si>
+    <t>FTILE761</t>
+  </si>
+  <si>
+    <t>ZAPORTAL</t>
+  </si>
+  <si>
+    <t>CONS1_5</t>
+  </si>
+  <si>
+    <t>ASHWALL2</t>
+  </si>
+  <si>
+    <t>TILE0830</t>
+  </si>
+  <si>
+    <t>NEW52</t>
+  </si>
+  <si>
+    <t>NEW33</t>
+  </si>
+  <si>
+    <t>NUKAGE1</t>
+  </si>
+  <si>
+    <t>NONE</t>
+  </si>
+  <si>
+    <t>FLOOR4_1</t>
+  </si>
+  <si>
+    <t>OUTC60</t>
+  </si>
+  <si>
+    <t>NEW80</t>
+  </si>
+  <si>
+    <t>NEW29</t>
+  </si>
+  <si>
+    <t>TILE02F6</t>
+  </si>
+  <si>
+    <t>OUTC45</t>
+  </si>
+  <si>
+    <t>NEW91</t>
+  </si>
+  <si>
+    <t>TILE1436</t>
+  </si>
+  <si>
+    <t>TILED7C9</t>
+  </si>
+  <si>
+    <t>FWATER1</t>
+  </si>
+  <si>
+    <t>TILE33A7</t>
+  </si>
+  <si>
+    <t>BLOOD1</t>
+  </si>
+  <si>
+    <t>RROCK05</t>
+  </si>
+  <si>
+    <t>NEW44</t>
+  </si>
+  <si>
+    <t>NEW83</t>
+  </si>
+  <si>
+    <t>TILE1CB1</t>
+  </si>
+  <si>
+    <t>NEW82</t>
+  </si>
+  <si>
+    <t>NEW18</t>
   </si>
 </sst>
 </file>
@@ -881,20 +965,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{764EE261-F28C-4A12-9150-B74128514BA4}">
-  <dimension ref="A1:E121"/>
+  <dimension ref="A1:E140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="D116" sqref="D116"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" customWidth="1"/>
-    <col min="3" max="4" width="16.28515625" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" customWidth="1"/>
+    <col min="1" max="1" width="21.5546875" customWidth="1"/>
+    <col min="3" max="4" width="16.33203125" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -909,841 +993,1001 @@
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>76</v>
-      </c>
-      <c r="D3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>71</v>
       </c>
       <c r="D5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>74</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C8" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>77</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C9" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>107</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C10" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>117</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C11" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>136</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C12" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>191</v>
+      </c>
+      <c r="C13" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>90</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C14" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>88</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C15" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>116</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C16" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>114</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C17" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>26</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C18" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>128</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C19" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>140</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C20" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>177</v>
+      </c>
+      <c r="C21" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>69</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C22" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>19</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C23" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>171</v>
+      </c>
+      <c r="C24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>24</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C25" t="s">
         <v>52</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D25" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>25</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C26" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>4</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C27" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>39</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C28" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>131</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C29" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>99</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C30" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>130</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C31" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>96</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C32" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>187</v>
+      </c>
+      <c r="C33" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>109</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C34" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>139</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C35" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
         <v>129</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C36" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
         <v>0</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C37" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>170</v>
+      </c>
+      <c r="C38" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>15</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C39" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>79</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C40" t="s">
         <v>82</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D40" t="s">
         <v>80</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E40" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
         <v>57</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C41" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
         <v>53</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C42" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>17</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C43" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
         <v>27</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C44" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
         <v>11</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C45" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
         <v>138</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C46" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>58</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C47" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
         <v>137</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C48" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>83</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C49" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
         <v>105</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C50" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
         <v>121</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C51" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
         <v>122</v>
-      </c>
-      <c r="C45" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>124</v>
-      </c>
-      <c r="C46" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>123</v>
-      </c>
-      <c r="C47" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>10</v>
-      </c>
-      <c r="C48" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>92</v>
-      </c>
-      <c r="D49" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>13</v>
-      </c>
-      <c r="C50" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>84</v>
-      </c>
-      <c r="C51" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>100</v>
       </c>
       <c r="C52" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
+        <v>124</v>
+      </c>
+      <c r="C53" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>176</v>
+      </c>
+      <c r="C54" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>123</v>
+      </c>
+      <c r="C55" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>190</v>
+      </c>
+      <c r="C56" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>10</v>
+      </c>
+      <c r="C57" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>92</v>
+      </c>
+      <c r="D58" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>13</v>
+      </c>
+      <c r="C59" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>84</v>
+      </c>
+      <c r="C60" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>100</v>
+      </c>
+      <c r="C61" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
         <v>102</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C62" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
         <v>104</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C63" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
         <v>94</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C64" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
         <v>103</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C65" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
         <v>95</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C66" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
         <v>141</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C67" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
         <v>143</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C68" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
         <v>144</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C69" t="s">
         <v>59</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D69" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
         <v>146</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D70" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>188</v>
+      </c>
+      <c r="C71" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>84</v>
+      </c>
+      <c r="C72" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>180</v>
+      </c>
+      <c r="D73" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
         <v>147</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C80" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
         <v>6</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C81" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
         <v>29</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C85" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
         <v>31</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C86" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
         <v>36</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C87" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
         <v>40</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C88" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
         <v>20</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C89" t="s">
         <v>52</v>
       </c>
-      <c r="D78" t="s">
+      <c r="D89" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
         <v>37</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C90" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
         <v>34</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C91" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
         <v>22</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C92" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
         <v>46</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C93" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
         <v>91</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C94" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
         <v>30</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C95" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
         <v>28</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C96" t="s">
         <v>52</v>
       </c>
-      <c r="D85" t="s">
+      <c r="D96" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
         <v>33</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C97" t="s">
         <v>52</v>
       </c>
-      <c r="D86" t="s">
+      <c r="D97" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
         <v>111</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C98" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
         <v>47</v>
       </c>
-      <c r="C93" t="s">
+      <c r="C104" t="s">
         <v>50</v>
       </c>
-      <c r="D93" t="s">
+      <c r="D104" t="s">
         <v>48</v>
       </c>
-      <c r="E93" t="s">
+      <c r="E104" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
         <v>127</v>
       </c>
-      <c r="C94" t="s">
+      <c r="C105" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
         <v>132</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C106" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
         <v>113</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C107" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
         <v>51</v>
       </c>
-      <c r="C97" t="s">
+      <c r="C108" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
         <v>60</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C109" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
         <v>67</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C110" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
         <v>64</v>
       </c>
-      <c r="C100" t="s">
+      <c r="C111" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
         <v>126</v>
       </c>
-      <c r="C101" t="s">
+      <c r="C112" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
         <v>55</v>
       </c>
-      <c r="C102" t="s">
+      <c r="C113" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
         <v>42</v>
       </c>
-      <c r="C103" t="s">
+      <c r="C114" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
         <v>8</v>
       </c>
-      <c r="C104" t="s">
+      <c r="C115" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
         <v>125</v>
       </c>
-      <c r="C105" t="s">
+      <c r="C116" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
         <v>86</v>
       </c>
-      <c r="C106" t="s">
+      <c r="C117" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
         <v>44</v>
       </c>
-      <c r="C107" t="s">
+      <c r="C118" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
         <v>66</v>
       </c>
-      <c r="C108" t="s">
+      <c r="C119" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
         <v>62</v>
       </c>
-      <c r="C109" t="s">
+      <c r="C120" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A112" s="1" t="s">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>165</v>
+      </c>
+      <c r="C122" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>167</v>
+      </c>
+      <c r="C123" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>168</v>
+      </c>
+      <c r="C124" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>169</v>
+      </c>
+      <c r="C125" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>174</v>
+      </c>
+      <c r="C126" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
+        <v>182</v>
+      </c>
+      <c r="C127" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>184</v>
+      </c>
+      <c r="C128" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>186</v>
+      </c>
+      <c r="C129" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A131" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
         <v>150</v>
       </c>
-      <c r="C114" t="s">
+      <c r="C133" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
         <v>151</v>
       </c>
-      <c r="C115" t="s">
+      <c r="C134" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
         <v>153</v>
       </c>
-      <c r="C116" t="s">
+      <c r="C135" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
         <v>155</v>
       </c>
-      <c r="C117" t="s">
+      <c r="C136" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
         <v>157</v>
       </c>
-      <c r="C118" t="s">
+      <c r="C137" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
         <v>159</v>
       </c>
-      <c r="C119" t="s">
+      <c r="C138" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
         <v>161</v>
       </c>
-      <c r="C120" t="s">
+      <c r="C139" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
         <v>163</v>
       </c>
-      <c r="C121" t="s">
+      <c r="C140" t="s">
         <v>164</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:E57">
-    <sortCondition ref="A3:A57"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:E66">
+    <sortCondition ref="A5:A66"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
REC07. tweakS to D64TM & D6434TC
D64TM - Corpse removal for test facility after arena reset.
D6434TC - Revised unmaker secret door.
</commit_message>
<xml_diff>
--- a/Reference_Info/Texture replacements.xlsx
+++ b/Reference_Info/Texture replacements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Connell\Documents\GitHub\BD64-VoH_maps\Reference_Info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD6AF085-C554-4998-B4D0-1FC36D4192FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7DA5640-7076-4703-A7E8-12669DE55C3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="2175" windowWidth="21600" windowHeight="11295" xr2:uid="{A567E191-AF02-4B5D-A98D-30E219FAA09A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A567E191-AF02-4B5D-A98D-30E219FAA09A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="213">
   <si>
     <t>NEW50</t>
   </si>
@@ -652,6 +652,21 @@
   </si>
   <si>
     <t>Blue Fireball</t>
+  </si>
+  <si>
+    <t>Orange Demon artefact</t>
+  </si>
+  <si>
+    <t>Secret Line Cross</t>
+  </si>
+  <si>
+    <t>LINE SPECIALS</t>
+  </si>
+  <si>
+    <t>Stimpack</t>
+  </si>
+  <si>
+    <t>Megasphere</t>
   </si>
 </sst>
 </file>
@@ -1024,10 +1039,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{764EE261-F28C-4A12-9150-B74128514BA4}">
-  <dimension ref="A1:E163"/>
+  <dimension ref="A1:E165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="D164" sqref="A159:D164"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="C161" sqref="C161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2075,7 +2090,7 @@
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="2">
-        <v>2024</v>
+        <v>556</v>
       </c>
       <c r="C148" t="s">
         <v>196</v>
@@ -2171,19 +2186,47 @@
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" s="2"/>
+      <c r="A159" s="2">
+        <v>4000</v>
+      </c>
+      <c r="C159" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" s="2"/>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A161" s="2"/>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A160" s="2">
+        <v>7582</v>
+      </c>
+      <c r="C160" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" s="2">
+        <v>554</v>
+      </c>
+      <c r="C161" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="2"/>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" s="2"/>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165" s="2">
+        <v>994</v>
+      </c>
+      <c r="C165" t="s">
+        <v>209</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:E66">

</xml_diff>

<commit_message>
REC08. D6402 & D6415 tweaks
D6402 - Changed blue key move timers and lights. Fake blue key removed.

D6415 - Simplified soulsphere puzzle script. Fake soulsphere removed.
</commit_message>
<xml_diff>
--- a/Reference_Info/Texture replacements.xlsx
+++ b/Reference_Info/Texture replacements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Connell\Documents\GitHub\BD64-VoH_maps\Reference_Info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7DA5640-7076-4703-A7E8-12669DE55C3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF32365-C0B3-4421-AD92-2EAE149AEC73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A567E191-AF02-4B5D-A98D-30E219FAA09A}"/>
+    <workbookView xWindow="7200" yWindow="2175" windowWidth="21600" windowHeight="11295" xr2:uid="{A567E191-AF02-4B5D-A98D-30E219FAA09A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="217">
   <si>
     <t>NEW50</t>
   </si>
@@ -667,6 +667,18 @@
   </si>
   <si>
     <t>Megasphere</t>
+  </si>
+  <si>
+    <t>Split Door</t>
+  </si>
+  <si>
+    <t>Teleport</t>
+  </si>
+  <si>
+    <t>TELEPORTMEDKIT</t>
+  </si>
+  <si>
+    <t>TELEPORTPAIN</t>
   </si>
 </sst>
 </file>
@@ -1039,10 +1051,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{764EE261-F28C-4A12-9150-B74128514BA4}">
-  <dimension ref="A1:E165"/>
+  <dimension ref="A1:E169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="C161" sqref="C161"/>
+    <sheetView tabSelected="1" topLeftCell="A151" workbookViewId="0">
+      <selection activeCell="C167" sqref="C167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2228,6 +2240,38 @@
         <v>209</v>
       </c>
     </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166" s="2">
+        <v>2087</v>
+      </c>
+      <c r="C166" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167" s="2">
+        <v>97</v>
+      </c>
+      <c r="C167" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168" s="2">
+        <v>7581</v>
+      </c>
+      <c r="C168" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169" s="2">
+        <v>7618</v>
+      </c>
+      <c r="C169" t="s">
+        <v>216</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:E66">
     <sortCondition ref="A5:A66"/>

</xml_diff>